<commit_message>
Iteracion 2 de lista de requisitos
</commit_message>
<xml_diff>
--- a/STU/Analisis y Diseño/STU_LR.xlsx
+++ b/STU/Analisis y Diseño/STU_LR.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ITERACION1" sheetId="1" r:id="rId1"/>
+    <sheet name="ITERACION2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -199,6 +200,36 @@
   </si>
   <si>
     <t>LISTA DE REQUISITOS DEL Sistema de transporte urbano</t>
+  </si>
+  <si>
+    <t>Caso de Uso</t>
+  </si>
+  <si>
+    <t>Prioridad</t>
+  </si>
+  <si>
+    <t>Prototipos</t>
+  </si>
+  <si>
+    <t>CU01-Busqueda de vehiculos</t>
+  </si>
+  <si>
+    <t>CU02-Mostrar informacion de propietario</t>
+  </si>
+  <si>
+    <t>CU03-Realizar comentarios</t>
+  </si>
+  <si>
+    <t>CU04-Realizar denuncia</t>
+  </si>
+  <si>
+    <t>CU05-Listar vehiculos top</t>
+  </si>
+  <si>
+    <t>CU06-Registrar infraccion</t>
+  </si>
+  <si>
+    <t>CU07-Pagar Infraccion</t>
   </si>
 </sst>
 </file>
@@ -236,15 +267,27 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -316,11 +359,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -329,36 +435,78 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -675,20 +823,20 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="8" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="50.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="50.85546875" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -696,7 +844,7 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="12"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -706,13 +854,13 @@
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -724,13 +872,13 @@
       <c r="C4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>45</v>
       </c>
     </row>
@@ -739,16 +887,16 @@
       <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="12" t="s">
         <v>46</v>
       </c>
     </row>
@@ -757,16 +905,16 @@
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="D6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="12" t="s">
         <v>47</v>
       </c>
     </row>
@@ -775,16 +923,16 @@
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="12" t="s">
         <v>48</v>
       </c>
     </row>
@@ -793,16 +941,16 @@
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="12" t="s">
         <v>49</v>
       </c>
     </row>
@@ -811,16 +959,16 @@
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="12" t="s">
         <v>50</v>
       </c>
     </row>
@@ -829,17 +977,17 @@
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>51</v>
+      <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -847,17 +995,17 @@
       <c r="B11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>52</v>
+      <c r="E11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -865,17 +1013,17 @@
       <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>53</v>
+      <c r="E12" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -883,17 +1031,17 @@
       <c r="B13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>54</v>
+      <c r="C13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -901,17 +1049,17 @@
       <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>55</v>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -919,17 +1067,17 @@
       <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>56</v>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -937,17 +1085,17 @@
       <c r="B16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>57</v>
+      <c r="D16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -955,17 +1103,17 @@
       <c r="B17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="10" t="s">
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>58</v>
+      <c r="E17" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -973,16 +1121,16 @@
       <c r="B18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="C18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="12" t="s">
         <v>46</v>
       </c>
     </row>
@@ -991,16 +1139,16 @@
       <c r="B19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="6" t="s">
+      <c r="C19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="12" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1009,17 +1157,17 @@
       <c r="B20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>46</v>
+      <c r="C20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1027,17 +1175,17 @@
       <c r="B21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>47</v>
+      <c r="C21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1045,17 +1193,17 @@
       <c r="B22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>50</v>
+      <c r="C22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1063,17 +1211,17 @@
       <c r="B23" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>50</v>
+      <c r="C23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1083,4 +1231,536 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="42.140625" customWidth="1"/>
+    <col min="5" max="5" width="63" customWidth="1"/>
+    <col min="6" max="6" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="24">
+        <v>1</v>
+      </c>
+      <c r="H4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="32"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="22"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="22"/>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="22"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="27">
+        <v>4</v>
+      </c>
+      <c r="H10" s="29"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="20">
+        <v>5</v>
+      </c>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="24">
+        <v>3</v>
+      </c>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="22"/>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="28">
+        <v>2</v>
+      </c>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="24">
+        <v>5</v>
+      </c>
+      <c r="H16" s="21"/>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="22"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="23"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="25"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="26"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="H4:H9"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="G20:G23"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="G4:G9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Lista de Requisitos : Modificacion de requisitos CU4
</commit_message>
<xml_diff>
--- a/STU/Analisis y Diseño/STU_LR.xlsx
+++ b/STU/Analisis y Diseño/STU_LR.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPJA\STU\Analisis y Diseño\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -459,12 +454,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -474,6 +463,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -492,19 +500,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -568,7 +563,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -603,7 +598,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -830,13 +825,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -875,7 +870,7 @@
       <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="11" t="s">
@@ -893,7 +888,7 @@
       <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="17" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="12" t="s">
@@ -911,7 +906,7 @@
       <c r="D6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="17" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="12" t="s">
@@ -929,7 +924,7 @@
       <c r="D7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="17" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="12" t="s">
@@ -947,7 +942,7 @@
       <c r="D8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="17" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -965,7 +960,7 @@
       <c r="D9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="17" t="s">
         <v>35</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -983,7 +978,7 @@
       <c r="D10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="12" t="s">
@@ -1001,7 +996,7 @@
       <c r="D11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F11" s="12" t="s">
@@ -1019,7 +1014,7 @@
       <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="17" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="12" t="s">
@@ -1037,7 +1032,7 @@
       <c r="D13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="17" t="s">
         <v>38</v>
       </c>
       <c r="F13" s="12" t="s">
@@ -1055,7 +1050,7 @@
       <c r="D14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F14" s="12" t="s">
@@ -1073,7 +1068,7 @@
       <c r="D15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="17" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="12" t="s">
@@ -1091,7 +1086,7 @@
       <c r="D16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="12" t="s">
@@ -1109,7 +1104,7 @@
       <c r="D17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="17" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="12" t="s">
@@ -1127,7 +1122,7 @@
       <c r="D18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="17" t="s">
         <v>31</v>
       </c>
       <c r="F18" s="12" t="s">
@@ -1145,7 +1140,7 @@
       <c r="D19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="17" t="s">
         <v>32</v>
       </c>
       <c r="F19" s="12" t="s">
@@ -1163,7 +1158,7 @@
       <c r="D20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="17" t="s">
         <v>29</v>
       </c>
       <c r="F20" s="12" t="s">
@@ -1181,7 +1176,7 @@
       <c r="D21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="17" t="s">
         <v>44</v>
       </c>
       <c r="F21" s="12" t="s">
@@ -1199,7 +1194,7 @@
       <c r="D22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="17" t="s">
         <v>31</v>
       </c>
       <c r="F22" s="12" t="s">
@@ -1217,7 +1212,7 @@
       <c r="D23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="17" t="s">
         <v>32</v>
       </c>
       <c r="F23" s="12" t="s">
@@ -1238,7 +1233,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1254,13 +1249,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
@@ -1285,13 +1280,13 @@
       <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1305,7 +1300,7 @@
       <c r="C4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -1314,10 +1309,10 @@
       <c r="F4" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="29">
         <v>1</v>
       </c>
-      <c r="H4" s="21"/>
+      <c r="H4" s="26"/>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1329,15 +1324,15 @@
       <c r="C5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="17" t="s">
         <v>31</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>46</v>
       </c>
       <c r="F5" s="32"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="22"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1349,15 +1344,15 @@
       <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="17" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>47</v>
       </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="22"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="27"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1369,15 +1364,15 @@
       <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="17" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="32"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="22"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1389,15 +1384,15 @@
       <c r="C8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="32"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="22"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="27"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -1409,15 +1404,15 @@
       <c r="C9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="17" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>50</v>
       </c>
       <c r="F9" s="32"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="23"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1429,19 +1424,19 @@
       <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="19">
         <v>4</v>
       </c>
-      <c r="H10" s="29"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1453,19 +1448,19 @@
       <c r="C11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="17" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="F11" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="18">
         <v>5</v>
       </c>
-      <c r="H11" s="18"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1477,7 +1472,7 @@
       <c r="C12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="17" t="s">
         <v>37</v>
       </c>
       <c r="E12" s="12" t="s">
@@ -1486,10 +1481,10 @@
       <c r="F12" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="29">
         <v>3</v>
       </c>
-      <c r="H12" s="21"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1501,15 +1496,15 @@
       <c r="C13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>53</v>
       </c>
       <c r="F13" s="32"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="22"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="27"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1521,17 +1516,17 @@
       <c r="C14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>42</v>
+      <c r="D14" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F14" s="32"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="23"/>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G14" s="31"/>
+      <c r="H14" s="28"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1541,21 +1536,21 @@
       <c r="C15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>39</v>
+      <c r="D15" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="20">
         <v>2</v>
       </c>
-      <c r="H15" s="18"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="H15" s="16"/>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -1563,23 +1558,23 @@
         <v>28</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>40</v>
+        <v>25</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="29">
         <v>5</v>
       </c>
-      <c r="H16" s="21"/>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
@@ -1587,17 +1582,17 @@
         <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="22"/>
+        <v>46</v>
+      </c>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="27"/>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -1609,15 +1604,15 @@
       <c r="C18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>31</v>
+      <c r="D18" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="22"/>
+        <v>47</v>
+      </c>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="27"/>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -1629,17 +1624,17 @@
       <c r="C19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="19" t="s">
-        <v>32</v>
+      <c r="D19" s="17" t="s">
+        <v>29</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="23"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="28"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
@@ -1647,21 +1642,21 @@
         <v>29</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>22</v>
       </c>
@@ -1669,17 +1664,17 @@
         <v>29</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
+        <v>46</v>
+      </c>
+      <c r="F21" s="30"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1691,15 +1686,15 @@
       <c r="C22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
+      <c r="D22" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="30"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1708,45 +1703,39 @@
       <c r="B23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="G4:G9"/>
     <mergeCell ref="H16:H19"/>
     <mergeCell ref="H20:H23"/>
     <mergeCell ref="H4:H9"/>
@@ -1757,9 +1746,6 @@
     <mergeCell ref="G16:G19"/>
     <mergeCell ref="G20:G23"/>
     <mergeCell ref="H12:H14"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F4:F9"/>
-    <mergeCell ref="G4:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Lista de requisitos : Modificacion de prioridades
</commit_message>
<xml_diff>
--- a/STU/Analisis y Diseño/STU_LR.xlsx
+++ b/STU/Analisis y Diseño/STU_LR.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -482,6 +482,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,18 +502,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1230,10 +1230,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1306,13 +1306,13 @@
       <c r="E4" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="27">
         <v>1</v>
       </c>
-      <c r="H4" s="26"/>
+      <c r="H4" s="30"/>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1330,9 +1330,9 @@
       <c r="E5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="32"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="27"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1350,9 +1350,9 @@
       <c r="E6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="27"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1370,9 +1370,9 @@
       <c r="E7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="27"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="31"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1390,9 +1390,9 @@
       <c r="E8" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="27"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="31"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -1410,9 +1410,9 @@
       <c r="E9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="28"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="32"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1434,7 +1434,7 @@
         <v>64</v>
       </c>
       <c r="G10" s="19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10" s="21"/>
     </row>
@@ -1458,7 +1458,7 @@
         <v>65</v>
       </c>
       <c r="G11" s="18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11" s="16"/>
     </row>
@@ -1478,13 +1478,13 @@
       <c r="E12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="27">
         <v>3</v>
       </c>
-      <c r="H12" s="26"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1502,16 +1502,16 @@
       <c r="E13" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="27"/>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="F13" s="26"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>43</v>
@@ -1520,63 +1520,63 @@
         <v>39</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="28"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="20">
+        <v>2</v>
+      </c>
+      <c r="H14" s="16"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="20">
-        <v>2</v>
-      </c>
-      <c r="H15" s="16"/>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="27">
+        <v>6</v>
+      </c>
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="29">
-        <v>5</v>
-      </c>
-      <c r="H16" s="26"/>
+        <v>46</v>
+      </c>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>28</v>
@@ -1588,15 +1588,15 @@
         <v>31</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="27"/>
+        <v>47</v>
+      </c>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>28</v>
@@ -1608,57 +1608,59 @@
         <v>32</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="27"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="32"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="28"/>
-    </row>
-    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="30">
+        <v>7</v>
+      </c>
+      <c r="H19" s="30"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>44</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
+        <v>46</v>
+      </c>
+      <c r="F20" s="28"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>29</v>
@@ -1669,44 +1671,33 @@
       <c r="D21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="E21" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="D22" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="30"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="E22" s="23"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E23" s="23"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E24" s="23"/>
@@ -1721,31 +1712,25 @@
       <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E26" s="23"/>
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
       <c r="H26" s="23"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F4:F9"/>
     <mergeCell ref="G4:G9"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="H15:H18"/>
+    <mergeCell ref="H19:H22"/>
     <mergeCell ref="H4:H9"/>
-    <mergeCell ref="F16:F19"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="G12:G14"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="G20:G23"/>
-    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="F19:F22"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="H12:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CUS01 : Anhadiendo prototipos
</commit_message>
<xml_diff>
--- a/STU/Analisis y Diseño/STU_LR.xlsx
+++ b/STU/Analisis y Diseño/STU_LR.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -1232,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1506,7 +1506,7 @@
       <c r="G13" s="28"/>
       <c r="H13" s="31"/>
     </row>
-    <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>39</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>67</v>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1538,13 +1538,13 @@
         <v>28</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F15" s="27" t="s">
         <v>68</v>
@@ -1554,7 +1554,7 @@
       </c>
       <c r="H15" s="30"/>
     </row>
-    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1562,13 +1562,13 @@
         <v>28</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>41</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
@@ -1581,14 +1581,12 @@
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>43</v>
-      </c>
+      <c r="C17" s="7"/>
       <c r="D17" s="17" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
@@ -1608,13 +1606,13 @@
         <v>32</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
       <c r="H18" s="32"/>
     </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>21</v>
       </c>
@@ -1622,13 +1620,13 @@
         <v>29</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F19" s="27" t="s">
         <v>69</v>
@@ -1638,7 +1636,7 @@
       </c>
       <c r="H19" s="30"/>
     </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -1646,13 +1644,13 @@
         <v>29</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>44</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="F20" s="28"/>
       <c r="G20" s="31"/>
@@ -1671,8 +1669,8 @@
       <c r="D21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>47</v>
+      <c r="E21" s="12" t="s">
+        <v>46</v>
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="31"/>
@@ -1685,10 +1683,15 @@
       <c r="B22" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="C22" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="D22" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="23"/>
+      <c r="E22" s="22" t="s">
+        <v>47</v>
+      </c>
       <c r="F22" s="29"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
@@ -1712,9 +1715,7 @@
       <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
+      <c r="E26" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>

<commit_message>
STU_LR: revision de los requisitos 2da iteracion
</commit_message>
<xml_diff>
--- a/STU/Analisis y Diseño/STU_LR.xlsx
+++ b/STU/Analisis y Diseño/STU_LR.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\workspace\php\RPJA\STU\Analisis y Diseño\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="76">
   <si>
     <t>ID</t>
   </si>
@@ -225,6 +230,24 @@
   </si>
   <si>
     <t>CU07-Pagar Infraccion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El sistema debe permitir ingresar los datos (archivos como imágenes, video, audio, descripcion) de una denuncia y registrarlos. </t>
+  </si>
+  <si>
+    <t>Ingresar numero de placa</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir ingresar en un campo de texto el numero de placa</t>
+  </si>
+  <si>
+    <t>Buscar por numero de placa</t>
+  </si>
+  <si>
+    <t>Detectar numero de placa en imagen</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir buscar por numero de placa</t>
   </si>
 </sst>
 </file>
@@ -563,7 +586,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -598,7 +621,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1232,8 +1255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1301,10 +1324,10 @@
         <v>25</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="F4" s="26" t="s">
         <v>63</v>
@@ -1325,10 +1348,10 @@
         <v>43</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="28"/>
@@ -1385,7 +1408,7 @@
         <v>43</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>49</v>
@@ -1476,7 +1499,7 @@
         <v>37</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="F12" s="26" t="s">
         <v>66</v>
@@ -1583,10 +1606,10 @@
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="17" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
@@ -1667,10 +1690,10 @@
         <v>43</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="31"/>

</xml_diff>

<commit_message>
CUS , LR : Añadiendo prototipos
</commit_message>
<xml_diff>
--- a/STU/Analisis y Diseño/STU_LR.xlsx
+++ b/STU/Analisis y Diseño/STU_LR.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\workspace\php\RPJA\STU\Analisis y Diseño\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
@@ -15,12 +10,17 @@
     <sheet name="ITERACION1" sheetId="1" r:id="rId1"/>
     <sheet name="ITERACION2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="PCU03_">"3 Imagen"</definedName>
+    <definedName name="PCU04_">"5 Imagen"</definedName>
+    <definedName name="PCU05_">"7 Imagen"</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="83">
   <si>
     <t>ID</t>
   </si>
@@ -248,6 +248,27 @@
   </si>
   <si>
     <t>El sistema debe permitir buscar por numero de placa</t>
+  </si>
+  <si>
+    <t>PCU01</t>
+  </si>
+  <si>
+    <t>PCU02</t>
+  </si>
+  <si>
+    <t>PCU03</t>
+  </si>
+  <si>
+    <t>PCU04</t>
+  </si>
+  <si>
+    <t>PCU05</t>
+  </si>
+  <si>
+    <t>PCU07</t>
+  </si>
+  <si>
+    <t>PCU06</t>
   </si>
 </sst>
 </file>
@@ -305,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -440,11 +461,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -479,7 +520,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -492,13 +532,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -524,6 +564,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -541,6 +587,319 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1372242</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>144041</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="1 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="485775" y="17992725"/>
+          <a:ext cx="4601217" cy="8354591"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3721875</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>54750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>283962</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>103534</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="2 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10246500" y="17837925"/>
+          <a:ext cx="4382112" cy="8306959"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1471575</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>4725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3272443</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>82066</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="3 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5186325" y="17949825"/>
+          <a:ext cx="4610743" cy="8173591"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>107100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1324637</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>41568</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="4 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="295275" y="9470175"/>
+          <a:ext cx="4744112" cy="8192643"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1304850</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3277192</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>39178</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="5 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5019600" y="9239175"/>
+          <a:ext cx="4782217" cy="8259328"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3521775</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>140400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>464915</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>65342</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="6 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10046400" y="9341550"/>
+          <a:ext cx="4763165" cy="8183117"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1490550</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>23700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3319997</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>53409</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="7 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5205300" y="26550825"/>
+          <a:ext cx="4639322" cy="8125959"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -586,7 +945,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -621,7 +980,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -832,9 +1191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -848,13 +1205,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -893,7 +1250,7 @@
       <c r="D4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="11" t="s">
@@ -911,7 +1268,7 @@
       <c r="D5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>31</v>
       </c>
       <c r="F5" s="12" t="s">
@@ -929,7 +1286,7 @@
       <c r="D6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="12" t="s">
@@ -947,7 +1304,7 @@
       <c r="D7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="12" t="s">
@@ -965,7 +1322,7 @@
       <c r="D8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="16" t="s">
         <v>34</v>
       </c>
       <c r="F8" s="12" t="s">
@@ -983,7 +1340,7 @@
       <c r="D9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>35</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -1001,7 +1358,7 @@
       <c r="D10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="12" t="s">
@@ -1019,7 +1376,7 @@
       <c r="D11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>36</v>
       </c>
       <c r="F11" s="12" t="s">
@@ -1037,7 +1394,7 @@
       <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="16" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="12" t="s">
@@ -1055,7 +1412,7 @@
       <c r="D13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="16" t="s">
         <v>38</v>
       </c>
       <c r="F13" s="12" t="s">
@@ -1073,7 +1430,7 @@
       <c r="D14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>42</v>
       </c>
       <c r="F14" s="12" t="s">
@@ -1091,7 +1448,7 @@
       <c r="D15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="E15" s="16" t="s">
         <v>39</v>
       </c>
       <c r="F15" s="12" t="s">
@@ -1109,7 +1466,7 @@
       <c r="D16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="12" t="s">
@@ -1127,7 +1484,7 @@
       <c r="D17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="17" t="s">
+      <c r="E17" s="16" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="12" t="s">
@@ -1145,7 +1502,7 @@
       <c r="D18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="16" t="s">
         <v>31</v>
       </c>
       <c r="F18" s="12" t="s">
@@ -1163,7 +1520,7 @@
       <c r="D19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="16" t="s">
         <v>32</v>
       </c>
       <c r="F19" s="12" t="s">
@@ -1181,7 +1538,7 @@
       <c r="D20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="17" t="s">
+      <c r="E20" s="16" t="s">
         <v>29</v>
       </c>
       <c r="F20" s="12" t="s">
@@ -1199,7 +1556,7 @@
       <c r="D21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="16" t="s">
         <v>44</v>
       </c>
       <c r="F21" s="12" t="s">
@@ -1217,7 +1574,7 @@
       <c r="D22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="16" t="s">
         <v>31</v>
       </c>
       <c r="F22" s="12" t="s">
@@ -1235,7 +1592,7 @@
       <c r="D23" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="16" t="s">
         <v>32</v>
       </c>
       <c r="F23" s="12" t="s">
@@ -1255,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1272,13 +1629,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
@@ -1323,19 +1680,21 @@
       <c r="C4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>71</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="26">
         <v>1</v>
       </c>
-      <c r="H4" s="30"/>
+      <c r="H4" s="32" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1347,15 +1706,15 @@
       <c r="C5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>73</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="31"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="33"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1367,15 +1726,15 @@
       <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="31"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="33"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1387,15 +1746,15 @@
       <c r="C7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="16" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="31"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="33"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1407,15 +1766,15 @@
       <c r="C8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>74</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="31"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="33"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -1427,15 +1786,15 @@
       <c r="C9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>35</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="32"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="33"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1447,19 +1806,21 @@
       <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="18">
         <v>5</v>
       </c>
-      <c r="H10" s="21"/>
+      <c r="H10" s="22" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1471,19 +1832,21 @@
       <c r="C11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <v>4</v>
       </c>
-      <c r="H11" s="16"/>
+      <c r="H11" s="17" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1495,19 +1858,21 @@
       <c r="C12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>37</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="26">
         <v>3</v>
       </c>
-      <c r="H12" s="30"/>
+      <c r="H12" s="29" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1519,15 +1884,15 @@
       <c r="C13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>38</v>
       </c>
       <c r="E13" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="31"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="30"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1539,19 +1904,21 @@
       <c r="C14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="19">
         <v>2</v>
       </c>
-      <c r="H14" s="16"/>
+      <c r="H14" s="17" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -1563,19 +1930,21 @@
       <c r="C15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D15" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="26">
         <v>6</v>
       </c>
-      <c r="H15" s="30"/>
+      <c r="H15" s="29" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1587,15 +1956,15 @@
       <c r="C16" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>41</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="31"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1605,15 +1974,15 @@
         <v>28</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="16" t="s">
         <v>73</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="31"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="30"/>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -1625,15 +1994,15 @@
       <c r="C18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="32"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="31"/>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -1645,19 +2014,21 @@
       <c r="C19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="30">
+      <c r="G19" s="29">
         <v>7</v>
       </c>
-      <c r="H19" s="30"/>
+      <c r="H19" s="29" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -1669,15 +2040,15 @@
       <c r="C20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="16" t="s">
         <v>44</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -1689,15 +2060,15 @@
       <c r="C21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>73</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -1709,36 +2080,36 @@
       <c r="C22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="29"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E26" s="23"/>
+      <c r="E26" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1757,5 +2128,6 @@
     <mergeCell ref="H12:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
STU_LR: Correccion descripcion RQ07
</commit_message>
<xml_diff>
--- a/STU/Analisis y Diseño/STU_LR.xlsx
+++ b/STU/Analisis y Diseño/STU_LR.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\workspace\php\RPJA\STU\Analisis y Diseño\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\development\workspace\projects\RPJA\STU\Analisis y Diseño\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>PCU06</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir mostrar el detalle de la informacion del propietario como: datos personales, vehiculos, infracciones, etc.</t>
   </si>
 </sst>
 </file>
@@ -525,6 +528,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,9 +557,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1188,13 +1191,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
     </row>
     <row r="2" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -1596,7 +1599,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1612,13 +1615,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
@@ -1669,13 +1672,13 @@
       <c r="E4" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="26">
         <v>1</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="29" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1695,9 +1698,9 @@
       <c r="E5" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="29"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="30"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1715,9 +1718,9 @@
       <c r="E6" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="29"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1735,9 +1738,9 @@
       <c r="E7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="24"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="29"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -1755,9 +1758,9 @@
       <c r="E8" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="29"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
@@ -1775,9 +1778,9 @@
       <c r="E9" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="30"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="31"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -1793,7 +1796,7 @@
         <v>42</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>64</v>
@@ -1847,13 +1850,13 @@
       <c r="E12" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="26">
         <v>3</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="H12" s="29" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1873,9 +1876,9 @@
       <c r="E13" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="29"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="30"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -1919,13 +1922,13 @@
       <c r="E15" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="26">
         <v>6</v>
       </c>
-      <c r="H15" s="28" t="s">
+      <c r="H15" s="29" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1945,9 +1948,9 @@
       <c r="E16" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="29"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="30"/>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1963,9 +1966,9 @@
       <c r="E17" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="29"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="30"/>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -1983,9 +1986,9 @@
       <c r="E18" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="30"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="31"/>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -2003,13 +2006,13 @@
       <c r="E19" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="28">
+      <c r="G19" s="29">
         <v>7</v>
       </c>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="29" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2029,9 +2032,9 @@
       <c r="E20" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -2049,9 +2052,9 @@
       <c r="E21" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
@@ -2066,12 +2069,12 @@
       <c r="D22" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E23" s="20"/>

</xml_diff>